<commit_message>
get agent and circular import fix
</commit_message>
<xml_diff>
--- a/Employee System Integration Format/employees.xlsx
+++ b/Employee System Integration Format/employees.xlsx
@@ -602,37 +602,37 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>TE125</t>
+          <t>TE126</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ajay Menon</t>
+          <t>Mohammed Saneer</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Ajay</t>
+          <t>Mohammed</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Menon</t>
+          <t>Saneer</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>m.ajay@dynasas.com</t>
+          <t>saneer@dynasas.com</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>971508341694</t>
+          <t>971523235404</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -679,12 +679,12 @@
       <c r="AD2" t="inlineStr"/>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>ajaymeno</t>
+          <t>mohasane</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>a8169e82c094d6a27a9c344be69ac5ff10f2970655b2486d1f3fc72330b93141</t>
+          <t>c60019ad46409b66a812d6db61e2aa04f3ce644019d178761b5ef50e4af49db5</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
@@ -695,37 +695,37 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TE124</t>
+          <t>TE125</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ibrahim Rathwala</t>
+          <t>Ajay Menon</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ibrahim</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Rathwala</t>
+          <t>Menon</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>yobozyt@gmail.com</t>
+          <t>m.ajay@dynasas.com</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>971561093935</t>
+          <t>971508341694</t>
         </is>
       </c>
       <c r="I3" t="inlineStr"/>
@@ -772,12 +772,12 @@
       <c r="AD3" t="inlineStr"/>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>ibrarath</t>
+          <t>ajaymeno</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>c04510499ffc6d99ad1c1f402b14127e189257b19fa63f495da856bbff88db74</t>
+          <t>5aee76819f9b4633d11cd5abf7f8c2f6064ffa43e4cd72d1e091ef300d418008</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
@@ -788,37 +788,37 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TE126</t>
+          <t>TE124</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mohammed Saneer</t>
+          <t>Ibrahim Rathwala</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Mohammed</t>
+          <t>Ibrahim</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Saneer</t>
+          <t>Rathwala</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>saneer@dynasas.com</t>
+          <t>yobozyt@gmail.com</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>971523235404</t>
+          <t>971561093935</t>
         </is>
       </c>
       <c r="I4" t="inlineStr"/>
@@ -865,12 +865,12 @@
       <c r="AD4" t="inlineStr"/>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>mohasane</t>
+          <t>ibrarath</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>96f2fcdf8c75fd56086ff58227279f741db4d4b4e7fdbfaac4defd19980e1ae2</t>
+          <t>30426da7ae9b01536a5b2b9ed461c17a323861583bd75284bc90a48065589658</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
@@ -958,12 +958,12 @@
       <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>ahmameda</t>
+          <t>ahmameda47</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>578cd8b68810ba3e780b2c56d7837e4e52605a5e2cc41fc6265377097cbb55d4</t>
+          <t>9f573e54f8f4ec488c5c8646a9cd42972847c16809e79e81aa13c2aa1064f956</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
@@ -974,37 +974,37 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TE128</t>
+          <t>TE127</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ruhban Gill</t>
+          <t>Hamza Ameen</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ruhban</t>
+          <t>Hamza</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Gill</t>
+          <t>Ameen</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Ruhban@dynasas.com</t>
+          <t>ameen.h@dynasas.com</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>971554980651</t>
+          <t>971566237633</t>
         </is>
       </c>
       <c r="I6" t="inlineStr"/>
@@ -1051,12 +1051,12 @@
       <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>ruhbgill</t>
+          <t>hamzamee84</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>022f1a2d30cf667c91a4f791affaf5e009da405c53587976da515cc26e6bbb96</t>
+          <t>0dac17096b8e19a861230bdaafb6cf01a29c929c8a7b5ae61cb0a7c28275ed10</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1067,37 +1067,37 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TE127</t>
+          <t>TE128</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Hamza Ameen</t>
+          <t>Ruhban Gill</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Hamza</t>
+          <t>Ruhban</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ameen</t>
+          <t>Gill</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>ameen.h@dynasas.com</t>
+          <t>Ruhban@dynasas.com</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>971566237633</t>
+          <t>971554980651</t>
         </is>
       </c>
       <c r="I7" t="inlineStr"/>
@@ -1144,12 +1144,12 @@
       <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>hamzamee</t>
+          <t>ruhbgill</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>a75a8ee4eb603717832d6c10359373ec1ad1c63a87c2b3dcaa85d81fd46e9701</t>
+          <t>34011906c331ed74ba1e3333a2a64a1bc4876c541a9c83c0b2e99637f386a236</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">

</xml_diff>